<commit_message>
Update Motor shield BOM
</commit_message>
<xml_diff>
--- a/Rpi0/Motor Shield/Motor Shield - BOM.xlsx
+++ b/Rpi0/Motor Shield/Motor Shield - BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="Motor Shield" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>Reference</t>
   </si>
@@ -36,175 +36,190 @@
     <t xml:space="preserve"> Datasheet</t>
   </si>
   <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:CP_Elec_5x5.3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>&lt; 40V</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>10V</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q_PMOS_GDSD</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-223</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix:TerminalBlock_Phoenix_MPT-0,5-2-2.54_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Female</t>
+  </si>
+  <si>
+    <t>Connector_PinSocket_2.54mm:PinSocket_1x04_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>LD1117S50TR_SOT223</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>http://www.st.com/st-web-ui/static/active/en/resource/technical/document/datasheet/CD00000544.pdf</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x01_P2.54mm_Vertical</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>IFX9201</t>
-  </si>
-  <si>
-    <t>Rob:IFX9201</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>Rob:PCB_Terminal_1725656</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>Capacitors_SMD:C_0805</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>100uF</t>
-  </si>
-  <si>
-    <t>Capacitors_Tantalum_SMD:CP_Tantalum_Case-A_EIA-3216-18_Hand</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>&lt; 40V</t>
-  </si>
-  <si>
-    <t>Diodes_SMD:D_1206</t>
+    <t>IFX9201SG</t>
+  </si>
+  <si>
+    <t>Rob-5.0:IFX9201SG</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>10V</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>Resistors_SMD:R_0805</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q_PMOS_GDSD</t>
-  </si>
-  <si>
-    <t>TO_SOT_Packages_SMD:SOT-223</t>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RPI0-Template</t>
+  </si>
+  <si>
+    <t>Rob-5.0:RPi0_Template</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
   <si>
     <t>U3</t>
   </si>
   <si>
-    <t>PIC16(L)F1509-I/SO</t>
-  </si>
-  <si>
-    <t>Housings_SSOP:SSOP-20_5.3x7.2mm_Pitch0.65mm</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>R3</t>
+    <t>PIC16F1509-ISS</t>
+  </si>
+  <si>
+    <t>Package_SO:SSOP-20_5.3x7.2mm_P0.65mm</t>
+  </si>
+  <si>
+    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/41609A.pdf</t>
   </si>
   <si>
     <t>J2</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x02_Pitch2.54mm</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>LD1117S50TR_SOT223</t>
-  </si>
-  <si>
-    <t>TO_SOT_Packages_SMD:SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Conn_01x04</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x04_Pitch2.54mm</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RPi0</t>
-  </si>
-  <si>
-    <t>Rob:RPi0_Template</t>
-  </si>
-  <si>
-    <t>J7</t>
   </si>
 </sst>
 </file>
@@ -1014,12 +1029,12 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,332 +1053,359 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>470</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C23" t="s">
         <v>52</v>
       </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
       <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C28" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D31" t="s">
         <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>